<commit_message>
complete the data and data wrangling
</commit_message>
<xml_diff>
--- a/data/education_investment(2001-2023).xlsx
+++ b/data/education_investment(2001-2023).xlsx
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>总  计</t>
   </si>
   <si>
     <t>北京市</t>
-  </si>
-  <si>
-    <t>17L.16</t>
   </si>
   <si>
     <t>天津市</t>
@@ -1324,7 +1321,7 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -1508,8 +1505,8 @@
       <c r="D3" s="2">
         <v>138.59</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
+      <c r="E3" s="4">
+        <v>171.16</v>
       </c>
       <c r="F3" s="1">
         <v>208.42</v>
@@ -1571,7 +1568,7 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>43.48</v>
@@ -1645,7 +1642,7 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>103.35</v>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>59.41</v>
@@ -1793,7 +1790,7 @@
     </row>
     <row r="7" ht="28" spans="1:24">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>48.14</v>
@@ -1867,7 +1864,7 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>95.78</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>58.34</v>
@@ -2015,7 +2012,7 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>72.49</v>
@@ -2089,7 +2086,7 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>123.61</v>
@@ -2163,7 +2160,7 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>161.37</v>
@@ -2237,7 +2234,7 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>128.72</v>
@@ -2311,7 +2308,7 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>77.91</v>
@@ -2385,7 +2382,7 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>89.61</v>
@@ -2459,7 +2456,7 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>53.97</v>
@@ -2533,7 +2530,7 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>156.14</v>
@@ -2607,7 +2604,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>116.53</v>
@@ -2681,7 +2678,7 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>75.76</v>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>77.52</v>
@@ -2829,7 +2826,7 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>228.85</v>
@@ -2903,7 +2900,7 @@
     </row>
     <row r="22" ht="28" spans="1:24">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>68.61</v>
@@ -2977,7 +2974,7 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>14.17</v>
@@ -3051,7 +3048,7 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>44.77</v>
@@ -3125,7 +3122,7 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>106.55</v>
@@ -3199,7 +3196,7 @@
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>46.16</v>
@@ -3273,7 +3270,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>91.72</v>
@@ -3347,7 +3344,7 @@
     </row>
     <row r="28" ht="28" spans="1:24">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>9.59</v>
@@ -3421,7 +3418,7 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>58.7</v>
@@ -3495,7 +3492,7 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>41.41</v>
@@ -3569,7 +3566,7 @@
     </row>
     <row r="31" spans="1:24">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>13.07</v>
@@ -3643,7 +3640,7 @@
     </row>
     <row r="32" ht="28" spans="1:24">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>13.68</v>
@@ -3717,7 +3714,7 @@
     </row>
     <row r="33" ht="28" spans="1:24">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>56.74</v>

</xml_diff>